<commit_message>
Getting files necessary for V3
</commit_message>
<xml_diff>
--- a/V3/assignments.xlsx
+++ b/V3/assignments.xlsx
@@ -16,6 +16,9 @@
     <sheet name="Assignment 7 - While Loops" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Assignment 8 - Lists" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Assignment 9 - Solution" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Assignment 10 - Func Test" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Assignment 11 - Relations" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Assignment 12 - Adv Plot" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -594,6 +597,577 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>function_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>solution_file</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>test_inputs</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>function_exists</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>calculate_stats</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Function calculate_stats should exist</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test_function_solution</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>calculate_stats</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Test function with lists and arrays against solution</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>solutions/assignment10_solution.py</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[{'args': [[1, 2, 3, 4, 5]]}, {'args': [[10, 20, 30]]}, {'args': [np.array([5, 10, 15])]}]</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>function_not_called</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>np.mean</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Should NOT use np.mean - must calculate manually</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>function_not_called</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>numpy.mean</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Should NOT use numpy.mean</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>expected_value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>var1_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>var2_name</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>relationship</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>variable_value</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>x should be array of values</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>check_relationship</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>y should equal cos(π * x)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>lambda x: np.cos(np.pi * x)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>check_relationship</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>z should equal 2x + 1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>lambda x: 2*x + 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>variable_type</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>y should be a list or array</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>min_lines</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>function</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>min_length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>xlabel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ylabel</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>has_legend</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>has_grid</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>function_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>plot_created</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Should create a plot</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>check_multiple_lines</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Plot should have at least 2 lines</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>check_function_any_line</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>One line should be cos(2x) with at least 50 points</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>lambda x: np.cos(2*x)</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>50</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>plot_properties</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Plot should have proper labels and legend</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Trigonometric Functions</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>function_not_called</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Should NOT use np.linspace</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>np.linspace</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>function_not_called</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Should NOT use numpy.linspace</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>numpy.linspace</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Advanced plotting and functions
</commit_message>
<xml_diff>
--- a/V3/assignments.xlsx
+++ b/V3/assignments.xlsx
@@ -19,6 +19,10 @@
     <sheet name="Assignment 10 - Func Test" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Assignment 11 - Relations" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Assignment 12 - Adv Plot" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Assignment 13 - Array Size" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Assignment 14 - Plot Style" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Assignment 15 - Type Match" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Assignment 16 - Plot Soln" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -543,11 +547,7 @@
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Check that y is set to 20</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
@@ -572,16 +572,8 @@
           <t>sum_xy should equal 30</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Correct! sum_xy = x + y = 30</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>sum_xy should be the sum of x and y</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -607,11 +599,7 @@
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>The message variable should be a string (text in quotes)</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -629,11 +617,7 @@
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Remember to use the + operator for addition</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>+</t>
@@ -651,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,6 +684,11 @@
           <t>tolerance</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>match_any_prefix</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -726,6 +715,7 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -743,16 +733,8 @@
           <t>Test function with lists and arrays against solution</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Your calculate_stats function produces correct results!</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Your calculate_stats function does not match expected output</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>solutions/assignment10_solution.py</t>
@@ -766,6 +748,7 @@
       <c r="H3" t="n">
         <v>0.01</v>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -775,12 +758,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>np.mean</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Should NOT use np.mean - must calculate manually</t>
+          <t>Should NOT use mean() with any prefix (np.mean, numpy.mean, etc.)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -790,38 +773,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Do not use np.mean() - calculate the mean yourself</t>
+          <t>Do not use np.mean or any mean() function - calculate it manually</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>function_not_called</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>numpy.mean</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Should NOT use numpy.mean</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Do not use numpy.mean() - calculate manually</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -940,11 +902,7 @@
           <t>y should equal cos(pi * x)</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Correct! y = cos(pi * x)</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>y should be calculated as cos(pi * x) for each value in x</t>
@@ -1043,7 +1001,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1120,6 +1078,11 @@
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>function_name</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>match_any_prefix</t>
         </is>
       </c>
     </row>
@@ -1146,6 +1109,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1176,6 +1140,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1212,6 +1177,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1256,6 +1222,7 @@
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1265,17 +1232,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Should NOT use np.linspace</t>
+          <t>Should NOT use linspace with any prefix</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Good - you created x values without np.linspace!</t>
+          <t>Good - you created x values without linspace!</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Do not use np.linspace - create x values another way (e.g., list comprehension)</t>
+          <t>Do not use np.linspace or any linspace() - create x values another way</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1289,36 +1256,956 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>np.linspace</t>
+          <t>linspace</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>min_size</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>pass_feedback</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fail_feedback</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>exact_size</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>min_value</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>max_value</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>function_name</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>match_any_prefix</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>array_size</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>x_values</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>x_values should have at least 100 elements</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Good - your array has enough data points!</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Your x_values array needs at least 100 elements</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>array_size</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>small_sample</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>small_sample should have exactly 10 elements</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>small_sample must have exactly 10 elements</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>array_values_in_range</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>x_values</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>All x_values should be between 0 and 10</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>All values are within the expected range!</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Some values in x_values are outside the range [0, 10]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>array_values_in_range</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>probabilities</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Probabilities should be between 0 and 1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Probabilities must be between 0 and 1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>function_not_called</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Should NOT use linspace (any prefix)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>linspace</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>true</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>function_not_called</t>
+          <t>function_called</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Should use arange (any prefix like np.arange)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Use np.arange or similar to create your array</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>arange</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pass_feedback</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fail_feedback</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>expected_style</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>line_index</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>expected_width</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>expected_size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>plot_created</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Should create a plot</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>plot_has_xlabel</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Plot must have an x-axis label (any text)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Good - your plot has an x-axis label!</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Add an x-axis label using plt.xlabel()</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>plot_has_ylabel</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Plot must have a y-axis label (any text)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Good - your plot has a y-axis label!</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Add a y-axis label using plt.ylabel()</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>plot_has_title</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Plot must have a title (any text)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Add a title using plt.title()</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>plot_line_style</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>First line should be solid blue (b-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Correct - first line is solid blue!</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>First line should be solid blue. Use plt.plot(x, y, "b-")</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>b-</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>plot_has_line_style</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Should NOT use numpy.linspace</t>
+          <t>Plot should have a red dashed line (r--)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Add a red dashed line using "r--" style</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>r--</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>numpy.linspace</t>
-        </is>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>plot_has_line_style</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Plot should have green star markers (g*)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Add a line with green star markers using "g*" style</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>g*</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>plot_line_width</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>First line should have width 2.0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Set the first line width to 2.0 using linewidth=2.0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>plot_marker_size</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Third line markers should be size 10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Set marker size to 10 using markersize=10</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>solution_file</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variables_to_compare</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>require_same_type</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>pass_feedback</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>fail_feedback</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>variable_name</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>expected_value</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>min_size</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>compare_solution</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>solutions/assignment15_solution.py</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>result_list, result_array</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Compare with solution - types must match exactly</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>All variables match with correct types!</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Variables must match AND be the same type (list vs numpy array)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>variable_type</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>result_list must be a Python list</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>result_list should be a Python list, not a numpy array</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>result_list</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>array_size</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>result_array should have at least 50 elements</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>result_array</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>pass_feedback</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fail_feedback</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>solution_file</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>line_index</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>check_color</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>check_linestyle</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>check_linewidth</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>check_marker</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>check_markersize</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>min_lines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>plot_created</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Should create a plot</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>compare_plot_solution</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Line 0 style should match solution</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Your plot styling matches the solution!</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Your line color, style, or width differs from the solution</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>solutions/assignment16_solution.py</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>check_multiple_lines</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Should have at least 2 lines</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1403,10 +2290,14 @@
           <t>Should use a for loop</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Good use of a for loop!</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>This assignment requires using a for loop</t>
+          <t>You need to use a for loop for this assignment</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1428,11 +2319,7 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Include an if statement in your code</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -1452,11 +2339,7 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Use the += operator to increment values</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>+=</t>
@@ -1514,11 +2397,7 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>The total should be the sum of numbers 0 through 99</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -1612,11 +2491,7 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Define a function named calculate_average</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -1638,11 +2513,7 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Define a function named find_maximum</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -1664,11 +2535,7 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Make sure to call calculate_average() in your code</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -1686,11 +2553,7 @@
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>The average of [1,2,3,4,5,6,7,8,9,10] should be 5.5</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
           <t>avg_result</t>
@@ -1791,11 +2654,7 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Use np.mean() to calculate the mean</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -1819,11 +2678,7 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Use np.std() to calculate standard deviation</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -1843,11 +2698,7 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Add "import numpy as np" at the top of your file</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>import numpy</t>
@@ -2011,11 +2862,7 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Use plt.plot() to create your line plot</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -2040,11 +2887,7 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Add an x-axis label with plt.xlabel()</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -2069,11 +2912,7 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Add a y-axis label with plt.ylabel()</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
@@ -2098,11 +2937,7 @@
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Add a title with plt.title()</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -2123,11 +2958,7 @@
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Your code should create a matplotlib plot</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -2147,16 +2978,8 @@
           <t>Plot should have correct labels and properties</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>All plot properties are correct!</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Check your plot title, labels, legend, and grid settings</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>Data Visualization</t>
@@ -2197,11 +3020,7 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Generate at least 50 data points for your plot</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
@@ -2294,11 +3113,7 @@
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Use the .format() method for string formatting</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -2350,11 +3165,7 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Use {} as placeholders in your format string</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
     </row>
@@ -2426,11 +3237,7 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>This assignment requires a while loop, not a for loop</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -2468,11 +3275,7 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Your while loop should run exactly 10 times</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
@@ -2601,11 +3404,7 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>my_list should be [1, 2, 3, 4, 5] in that exact order</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
     </row>
@@ -2712,7 +3511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2743,20 +3542,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>require_same_type</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>description</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>pass_feedback</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>fail_feedback</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>function_name</t>
         </is>
@@ -2783,20 +3587,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>Compare key variables with solution file</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Your solution matches the expected output!</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Your variable values differ from the expected solution</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2807,14 +3616,15 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Function process_data should exist</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
         <is>
           <t>process_data</t>
         </is>
@@ -2829,14 +3639,15 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Should use a for loop</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>